<commit_message>
Modefied Space budgeting to 4K
</commit_message>
<xml_diff>
--- a/Predictor_Comparison.xlsx
+++ b/Predictor_Comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d100503414d3fb8b/DOCUME-1/MobaXterm/slash/cvssa_desktopid0f9ke/RemoteFiles/1050764_2_9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d100503414d3fb8b/DOCUME-4/MobaXterm/slash/cvssa_desktopid0f9ke/RemoteFiles/1050764_2_12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{3948B1BC-FA4D-4D12-8844-ABE3CA4C13B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40C8BC9E-C8B0-4E1A-AD02-75F968865363}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{3948B1BC-FA4D-4D12-8844-ABE3CA4C13B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B06B6E00-20B4-478E-9E26-019B7912892B}"/>
   <bookViews>
-    <workbookView xWindow="-15240" yWindow="3435" windowWidth="13005" windowHeight="11385" xr2:uid="{C6F306F0-02D3-48EF-8207-115AB8E0274E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6F306F0-02D3-48EF-8207-115AB8E0274E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>INT-1</t>
   </si>
@@ -99,10 +99,7 @@
     <t>Alpha_Enhance</t>
   </si>
   <si>
-    <t>Hierarchical</t>
-  </si>
-  <si>
-    <t>Competetion</t>
+    <t>Competetion Predictor</t>
   </si>
 </sst>
 </file>
@@ -152,7 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -170,6 +169,1378 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alpha</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>INT-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>INT-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INT-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INT-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>INT-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FP-1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FP-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FP-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FP-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FP-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MM-1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>MM-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>MM-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MM-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MM-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>SERV-1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>SERV-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>SERV-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>SERV-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SERV-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.6189999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.840999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.625999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.325</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3979999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.3699999999999992</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.231999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4910000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.0129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.300999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.073</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.8439999999999994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.834</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17.167999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-763C-41D0-84CE-801570EC6A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alpha_Enhance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>INT-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>INT-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INT-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INT-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>INT-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FP-1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FP-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FP-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FP-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FP-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MM-1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>MM-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>MM-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MM-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MM-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>SERV-1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>SERV-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>SERV-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>SERV-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SERV-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.659000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3090000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.976000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8310000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.814</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.738</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.8350000000000009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.216000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17.585000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-763C-41D0-84CE-801570EC6A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Competetion Predictor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>INT-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>INT-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INT-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INT-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>INT-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FP-1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FP-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FP-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FP-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FP-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MM-1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>MM-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>MM-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>MM-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MM-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>SERV-1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>SERV-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>SERV-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>SERV-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SERV-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.794</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.929</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.966</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.592000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.048999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6739999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.484</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.356</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.0090000000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.255000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-763C-41D0-84CE-801570EC6A09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1727166560"/>
+        <c:axId val="1991027872"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1727166560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1991027872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1991027872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1727166560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6496FD2B-C5B4-432D-925F-B68420E25832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,19 +1840,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC56504-D39C-44F3-BDFC-F76F932E3787}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+      <selection sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>20</v>
       </c>
@@ -491,371 +1862,305 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>7.6189999999999998</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>7.383</v>
       </c>
       <c r="D2">
-        <v>6.5039999999999996</v>
-      </c>
-      <c r="E2">
-        <v>2.2690000000000001</v>
+        <v>4.835</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>10.840999999999999</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>10.659000000000001</v>
       </c>
       <c r="D3" s="1">
-        <v>7.798</v>
-      </c>
-      <c r="E3" s="1">
-        <v>13.976000000000001</v>
+        <v>11.509</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>12.625999999999999</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>13.153</v>
       </c>
       <c r="D4" s="1">
-        <v>12.348000000000001</v>
-      </c>
-      <c r="E4" s="1">
-        <v>17.881</v>
+        <v>16.794</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>2.4830000000000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2.3090000000000002</v>
       </c>
       <c r="D5">
-        <v>2.4449999999999998</v>
-      </c>
-      <c r="E5">
-        <v>1.522</v>
+        <v>1.929</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>0.41199999999999998</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.39300000000000002</v>
       </c>
       <c r="D6">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="E6">
-        <v>0.32500000000000001</v>
+        <v>0.34699999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>3.3119999999999998</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>3.1779999999999999</v>
       </c>
       <c r="D7">
-        <v>2.528</v>
-      </c>
-      <c r="E7">
-        <v>2.0569999999999999</v>
+        <v>2.5449999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>1.325</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>1.1339999999999999</v>
       </c>
       <c r="D8">
-        <v>1.3819999999999999</v>
-      </c>
-      <c r="E8">
-        <v>1.905</v>
+        <v>1.966</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.47599999999999998</v>
       </c>
       <c r="D9">
-        <v>0.67200000000000004</v>
-      </c>
-      <c r="E9">
-        <v>0.38500000000000001</v>
+        <v>0.43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>0.31</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.26600000000000001</v>
       </c>
       <c r="D10">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="E10">
-        <v>0.159</v>
+        <v>0.158</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>1.3979999999999999</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.33400000000000002</v>
       </c>
       <c r="D11">
-        <v>1.853</v>
-      </c>
-      <c r="E11">
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>8.3699999999999992</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>8.17</v>
       </c>
       <c r="D12" s="1">
-        <v>21.285</v>
-      </c>
-      <c r="E12" s="1">
-        <v>11.448</v>
+        <v>11.592000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>11.231999999999999</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>10.976000000000001</v>
       </c>
       <c r="D13" s="1">
-        <v>71.832999999999998</v>
-      </c>
-      <c r="E13" s="1">
-        <v>13.606999999999999</v>
+        <v>14.048999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>2.4910000000000001</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>2.2949999999999999</v>
       </c>
       <c r="D14">
-        <v>11.335000000000001</v>
-      </c>
-      <c r="E14">
-        <v>0.89200000000000002</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>2.2349999999999999</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>2.11</v>
       </c>
       <c r="D15">
-        <v>145.256</v>
-      </c>
-      <c r="E15">
-        <v>1.6759999999999999</v>
+        <v>1.6739999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>7.0129999999999999</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>6.8310000000000004</v>
       </c>
       <c r="D16" s="1">
-        <v>12.487</v>
-      </c>
-      <c r="E16" s="1">
-        <v>7.6269999999999998</v>
+        <v>7.16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>17.300999999999998</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>18.814</v>
       </c>
-      <c r="D17">
-        <v>26.004999999999999</v>
-      </c>
-      <c r="E17">
-        <v>12.802</v>
+      <c r="D17" s="1">
+        <v>11.484</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>18.073</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>19.738</v>
       </c>
-      <c r="D18">
-        <v>29.512</v>
-      </c>
-      <c r="E18">
-        <v>13.584</v>
+      <c r="D18" s="1">
+        <v>12.356</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <v>9.8439999999999994</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>9.8350000000000009</v>
       </c>
-      <c r="D19">
-        <v>27.759</v>
-      </c>
-      <c r="E19">
-        <v>9.8330000000000002</v>
+      <c r="D19" s="1">
+        <v>8.0090000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>15.834</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>16.216000000000001</v>
       </c>
-      <c r="D20">
-        <v>28.826000000000001</v>
-      </c>
-      <c r="E20">
-        <v>13.484</v>
+      <c r="D20" s="1">
+        <v>11.02</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>17.167999999999999</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>17.585000000000001</v>
       </c>
-      <c r="D21">
-        <v>30.545000000000002</v>
-      </c>
-      <c r="E21">
-        <v>14.044</v>
+      <c r="D21" s="1">
+        <v>11.255000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <f>SUM(B2:B21)</f>
         <v>150.41000000000003</v>
       </c>
-      <c r="C22">
-        <f t="shared" ref="C22:E22" si="0">SUM(C2:C21)</f>
+      <c r="C22" s="1">
+        <f t="shared" ref="C22" si="0">SUM(C2:C21)</f>
         <v>151.85500000000002</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>441.66000000000008</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>139.50699999999998</v>
+      <c r="D22" s="1">
+        <f>SUM(D2:D21)</f>
+        <v>129.84299999999999</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>